<commit_message>
Added login to PPM
</commit_message>
<xml_diff>
--- a/AddFixWorkPlanCost/Default.xlsx
+++ b/AddFixWorkPlanCost/Default.xlsx
@@ -520,13 +520,13 @@
     <col min="2" max="16384" width="9.1484375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row ht="12.75" customHeight="1" customFormat="1">
-      <c t="s">
+    <row r="1" ht="12.75" customHeight="1" customFormat="1">
+      <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row s="1" customFormat="1">
-      <c s="2" t="s">
+    <row r="2" s="1" customFormat="1">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
@@ -553,7 +553,7 @@
     <col min="1" max="16384" width="9.1484375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row ht="12.75" customHeight="1" customFormat="1"/>
+    <row r="1" ht="12.75" customHeight="1" customFormat="1"/>
   </sheetData>
   <printOptions gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>